<commit_message>
Changed naming from "grade book" to "customizable assignment report"
</commit_message>
<xml_diff>
--- a/gradebook.xlsx
+++ b/gradebook.xlsx
@@ -15,7 +15,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>StudentName</t>
+  </si>
+  <si>
+    <t>Franziska</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>GroupCount</t>
+  </si>
+  <si>
+    <t>sum_Correct</t>
+  </si>
+  <si>
+    <t>StudentName</t>
+  </si>
+  <si>
+    <t>Franziska</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Kathi</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Spandhana</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>GroupCount</t>
+  </si>
+  <si>
+    <t>mean_Score</t>
+  </si>
+  <si>
+    <t>new_mean_Score</t>
+  </si>
   <si>
     <t>StudentName</t>
   </si>
@@ -83,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -93,14 +141,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,25 +165,25 @@
   <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="true"/>
-    <col min="2" max="2" width="11.85546875" customWidth="true"/>
-    <col min="3" max="3" width="12.28515625" customWidth="true"/>
+    <col min="1" max="1" width="12.26953125" customWidth="true"/>
+    <col min="2" max="2" width="11.046875" customWidth="true"/>
+    <col min="3" max="3" width="11.6015625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0">
         <v>2</v>
@@ -142,7 +194,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -160,29 +212,29 @@
   <dimension ref="A1:D8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="true"/>
-    <col min="2" max="2" width="11.85546875" customWidth="true"/>
-    <col min="3" max="3" width="12" customWidth="true"/>
-    <col min="4" max="4" width="16.85546875" customWidth="true"/>
+    <col min="1" max="1" width="12.26953125" customWidth="true"/>
+    <col min="2" max="2" width="11.046875" customWidth="true"/>
+    <col min="3" max="3" width="11.26953125" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0">
         <v>2</v>
@@ -196,7 +248,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
@@ -210,7 +262,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0">
         <v>1</v>
@@ -224,7 +276,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0">
         <v>2</v>
@@ -238,7 +290,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0">
         <v>1</v>
@@ -252,7 +304,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0">
         <v>2</v>
@@ -266,7 +318,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0">
         <v>1</v>

</xml_diff>